<commit_message>
Atualiza base de usuários
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Downloads\Pr3cin5.0-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Downloads\PR3CIN - NOVO\Pr3cin5.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747596AA-32F2-4DDA-912E-EE3EAF79C3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D62319-0F46-4778-B819-207400C0DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8520AE5B-E2D7-423E-BB8E-26F01158B160}"/>
+    <workbookView xWindow="6060" yWindow="768" windowWidth="13596" windowHeight="11472" xr2:uid="{8520AE5B-E2D7-423E-BB8E-26F01158B160}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>usuario</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>1010baba</t>
+  </si>
+  <si>
+    <t>carlos</t>
+  </si>
+  <si>
+    <t>2020caca</t>
   </si>
 </sst>
 </file>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C1F19D-6CB6-470F-8155-5239829A4C32}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,6 +471,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>